<commit_message>
Finished excel parser, started with embrionic gui
</commit_message>
<xml_diff>
--- a/src/test/resources/sample_data/test_Leistungsnachweis_2017.xlsx
+++ b/src/test/resources/sample_data/test_Leistungsnachweis_2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1830" windowWidth="28800" windowHeight="12450" tabRatio="732"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="28800" windowHeight="12450" tabRatio="732"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="21" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="26">
   <si>
     <t>Summe 
 Total</t>
@@ -103,6 +103,12 @@
   <si>
     <t>11235 - Name 8</t>
   </si>
+  <si>
+    <t>Holidays</t>
+  </si>
+  <si>
+    <t>Overhead</t>
+  </si>
 </sst>
 </file>
 
@@ -113,7 +119,7 @@
     <numFmt numFmtId="165" formatCode="dd/"/>
     <numFmt numFmtId="166" formatCode="ddd"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1266,11 +1272,11 @@
   <dimension ref="A1:BN101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="1" customWidth="1"/>
@@ -1283,7 +1289,7 @@
     <col min="36" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="35.25" customHeight="1">
+    <row r="1" spans="1:66" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>4</v>
       </c>
@@ -1323,7 +1329,7 @@
       <c r="AG1" s="90"/>
       <c r="AH1" s="90"/>
     </row>
-    <row r="2" spans="1:66" ht="24.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:66" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="23"/>
@@ -1360,7 +1366,7 @@
       <c r="AH2" s="25"/>
       <c r="AI2" s="25"/>
     </row>
-    <row r="3" spans="1:66" ht="15.75" thickBot="1">
+    <row r="3" spans="1:66" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
@@ -1430,7 +1436,7 @@
       <c r="BM3" s="40"/>
       <c r="BN3" s="40"/>
     </row>
-    <row r="4" spans="1:66" ht="36.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:66" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="62">
         <v>42736</v>
       </c>
@@ -1473,7 +1479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:66" ht="25.5" thickBot="1">
+    <row r="5" spans="1:66" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="61" t="s">
         <v>5</v>
       </c>
@@ -1611,7 +1617,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:66" ht="26.45" customHeight="1" thickBot="1">
+    <row r="6" spans="1:66" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>14</v>
       </c>
@@ -1743,9 +1749,9 @@
       <c r="AH6" s="59"/>
       <c r="AI6" s="59"/>
     </row>
-    <row r="7" spans="1:66" ht="24" customHeight="1">
+    <row r="7" spans="1:66" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="33"/>
@@ -1787,9 +1793,9 @@
       </c>
       <c r="AI7" s="95"/>
     </row>
-    <row r="8" spans="1:66" ht="24" customHeight="1">
+    <row r="8" spans="1:66" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="33"/>
@@ -1831,7 +1837,7 @@
       </c>
       <c r="AI8" s="96"/>
     </row>
-    <row r="9" spans="1:66" ht="24" customHeight="1">
+    <row r="9" spans="1:66" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="32"/>
       <c r="C9" s="33"/>
@@ -1871,7 +1877,7 @@
       </c>
       <c r="AI9" s="96"/>
     </row>
-    <row r="10" spans="1:66" ht="24" customHeight="1">
+    <row r="10" spans="1:66" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="32"/>
       <c r="C10" s="33"/>
@@ -1911,7 +1917,7 @@
       </c>
       <c r="AI10" s="96"/>
     </row>
-    <row r="11" spans="1:66" ht="24" customHeight="1">
+    <row r="11" spans="1:66" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
       <c r="B11" s="32"/>
       <c r="C11" s="33"/>
@@ -1951,7 +1957,7 @@
       </c>
       <c r="AI11" s="96"/>
     </row>
-    <row r="12" spans="1:66" ht="24" customHeight="1">
+    <row r="12" spans="1:66" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="51"/>
       <c r="C12" s="33"/>
@@ -1991,7 +1997,7 @@
       </c>
       <c r="AI12" s="96"/>
     </row>
-    <row r="13" spans="1:66" ht="24" customHeight="1" thickBot="1">
+    <row r="13" spans="1:66" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
         <v>11</v>
       </c>
@@ -2033,7 +2039,7 @@
       </c>
       <c r="AI13" s="96"/>
     </row>
-    <row r="14" spans="1:66" ht="24" customHeight="1">
+    <row r="14" spans="1:66" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
         <v>13</v>
       </c>
@@ -2077,7 +2083,7 @@
       </c>
       <c r="AI14" s="96"/>
     </row>
-    <row r="15" spans="1:66" ht="24" customHeight="1">
+    <row r="15" spans="1:66" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
         <v>12</v>
       </c>
@@ -2119,7 +2125,7 @@
       </c>
       <c r="AI15" s="96"/>
     </row>
-    <row r="16" spans="1:66" ht="24" customHeight="1">
+    <row r="16" spans="1:66" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="32"/>
       <c r="C16" s="33"/>
@@ -2159,7 +2165,7 @@
       </c>
       <c r="AI16" s="96"/>
     </row>
-    <row r="17" spans="1:35" ht="24" customHeight="1">
+    <row r="17" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="32"/>
       <c r="C17" s="33"/>
@@ -2199,7 +2205,7 @@
       </c>
       <c r="AI17" s="96"/>
     </row>
-    <row r="18" spans="1:35" ht="24" customHeight="1">
+    <row r="18" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="32"/>
       <c r="C18" s="33"/>
@@ -2239,7 +2245,7 @@
       </c>
       <c r="AI18" s="96"/>
     </row>
-    <row r="19" spans="1:35" ht="24" customHeight="1">
+    <row r="19" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="32"/>
       <c r="C19" s="33"/>
@@ -2279,7 +2285,7 @@
       </c>
       <c r="AI19" s="96"/>
     </row>
-    <row r="20" spans="1:35" ht="24" customHeight="1">
+    <row r="20" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="51"/>
       <c r="C20" s="33"/>
@@ -2319,7 +2325,7 @@
       </c>
       <c r="AI20" s="96"/>
     </row>
-    <row r="21" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="21" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
         <v>15</v>
       </c>
@@ -2361,7 +2367,7 @@
       </c>
       <c r="AI21" s="96"/>
     </row>
-    <row r="22" spans="1:35" ht="24.75" customHeight="1">
+    <row r="22" spans="1:35" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>16</v>
       </c>
@@ -2409,7 +2415,7 @@
       </c>
       <c r="AI22" s="96"/>
     </row>
-    <row r="23" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="23" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="43" t="s">
         <v>10</v>
@@ -2453,7 +2459,7 @@
       </c>
       <c r="AI23" s="96"/>
     </row>
-    <row r="24" spans="1:35" ht="24" customHeight="1">
+    <row r="24" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>17</v>
       </c>
@@ -2499,7 +2505,7 @@
       </c>
       <c r="AI24" s="96"/>
     </row>
-    <row r="25" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="25" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
       <c r="B25" s="43" t="s">
         <v>10</v>
@@ -2545,7 +2551,7 @@
       </c>
       <c r="AI25" s="96"/>
     </row>
-    <row r="26" spans="1:35" ht="24" customHeight="1">
+    <row r="26" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
         <v>18</v>
       </c>
@@ -2591,7 +2597,7 @@
       </c>
       <c r="AI26" s="96"/>
     </row>
-    <row r="27" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="27" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27" s="43" t="s">
         <v>10</v>
@@ -2635,7 +2641,7 @@
       </c>
       <c r="AI27" s="96"/>
     </row>
-    <row r="28" spans="1:35" ht="24" customHeight="1">
+    <row r="28" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="30"/>
       <c r="B28" s="44"/>
       <c r="C28" s="48"/>
@@ -2675,7 +2681,7 @@
       </c>
       <c r="AI28" s="96"/>
     </row>
-    <row r="29" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="29" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
       <c r="B29" s="43"/>
       <c r="C29" s="48"/>
@@ -2715,7 +2721,7 @@
       </c>
       <c r="AI29" s="96"/>
     </row>
-    <row r="30" spans="1:35" ht="24" customHeight="1">
+    <row r="30" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30"/>
       <c r="B30" s="44"/>
       <c r="C30" s="48"/>
@@ -2755,7 +2761,7 @@
       </c>
       <c r="AI30" s="96"/>
     </row>
-    <row r="31" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="31" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="B31" s="43"/>
       <c r="C31" s="48"/>
@@ -2795,7 +2801,7 @@
       </c>
       <c r="AI31" s="96"/>
     </row>
-    <row r="32" spans="1:35" ht="24" customHeight="1">
+    <row r="32" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="45"/>
       <c r="B32" s="44"/>
       <c r="C32" s="48"/>
@@ -2835,7 +2841,7 @@
       </c>
       <c r="AI32" s="96"/>
     </row>
-    <row r="33" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="33" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
       <c r="B33" s="43"/>
       <c r="C33" s="48"/>
@@ -2875,7 +2881,7 @@
       </c>
       <c r="AI33" s="96"/>
     </row>
-    <row r="34" spans="1:35" ht="24" customHeight="1">
+    <row r="34" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="45"/>
       <c r="B34" s="44"/>
       <c r="C34" s="48"/>
@@ -2915,7 +2921,7 @@
       </c>
       <c r="AI34" s="96"/>
     </row>
-    <row r="35" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="35" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
       <c r="B35" s="53"/>
       <c r="C35" s="48"/>
@@ -2955,7 +2961,7 @@
       </c>
       <c r="AI35" s="96"/>
     </row>
-    <row r="36" spans="1:35" ht="24" customHeight="1">
+    <row r="36" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="49"/>
       <c r="B36" s="44"/>
       <c r="C36" s="48"/>
@@ -2995,7 +3001,7 @@
       </c>
       <c r="AI36" s="96"/>
     </row>
-    <row r="37" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="37" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="B37" s="53"/>
       <c r="C37" s="48"/>
@@ -3035,7 +3041,7 @@
       </c>
       <c r="AI37" s="96"/>
     </row>
-    <row r="38" spans="1:35" ht="24" customHeight="1">
+    <row r="38" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="45"/>
       <c r="B38" s="44"/>
       <c r="C38" s="48"/>
@@ -3075,7 +3081,7 @@
       </c>
       <c r="AI38" s="96"/>
     </row>
-    <row r="39" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="39" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="53"/>
       <c r="C39" s="48"/>
@@ -3115,7 +3121,7 @@
       </c>
       <c r="AI39" s="96"/>
     </row>
-    <row r="40" spans="1:35" ht="24" customHeight="1">
+    <row r="40" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="13"/>
       <c r="B40" s="44"/>
       <c r="C40" s="48"/>
@@ -3155,7 +3161,7 @@
       </c>
       <c r="AI40" s="96"/>
     </row>
-    <row r="41" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="41" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31"/>
       <c r="B41" s="53"/>
       <c r="C41" s="48"/>
@@ -3195,7 +3201,7 @@
       </c>
       <c r="AI41" s="96"/>
     </row>
-    <row r="42" spans="1:35" ht="24" customHeight="1">
+    <row r="42" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13"/>
       <c r="B42" s="44"/>
       <c r="C42" s="48"/>
@@ -3235,7 +3241,7 @@
       </c>
       <c r="AI42" s="96"/>
     </row>
-    <row r="43" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="43" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31"/>
       <c r="B43" s="43"/>
       <c r="C43" s="48"/>
@@ -3275,7 +3281,7 @@
       </c>
       <c r="AI43" s="96"/>
     </row>
-    <row r="44" spans="1:35" ht="24" customHeight="1">
+    <row r="44" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="30"/>
       <c r="B44" s="44"/>
       <c r="C44" s="48"/>
@@ -3315,7 +3321,7 @@
       </c>
       <c r="AI44" s="96"/>
     </row>
-    <row r="45" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="45" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="43"/>
       <c r="C45" s="48"/>
@@ -3355,7 +3361,7 @@
       </c>
       <c r="AI45" s="96"/>
     </row>
-    <row r="46" spans="1:35" ht="24" customHeight="1">
+    <row r="46" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="49"/>
       <c r="B46" s="44"/>
       <c r="C46" s="48"/>
@@ -3395,7 +3401,7 @@
       </c>
       <c r="AI46" s="96"/>
     </row>
-    <row r="47" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="47" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="43"/>
       <c r="C47" s="48"/>
@@ -3435,7 +3441,7 @@
       </c>
       <c r="AI47" s="96"/>
     </row>
-    <row r="48" spans="1:35" ht="24" customHeight="1">
+    <row r="48" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="42"/>
       <c r="B48" s="44"/>
       <c r="C48" s="48"/>
@@ -3475,7 +3481,7 @@
       </c>
       <c r="AI48" s="96"/>
     </row>
-    <row r="49" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="49" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="43"/>
       <c r="C49" s="48"/>
@@ -3515,7 +3521,7 @@
       </c>
       <c r="AI49" s="96"/>
     </row>
-    <row r="50" spans="1:35" ht="24" customHeight="1">
+    <row r="50" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
       <c r="B50" s="30"/>
       <c r="C50" s="48"/>
@@ -3555,7 +3561,7 @@
       </c>
       <c r="AI50" s="96"/>
     </row>
-    <row r="51" spans="1:35" ht="24" customHeight="1">
+    <row r="51" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="48"/>
@@ -3595,7 +3601,7 @@
       </c>
       <c r="AI51" s="96"/>
     </row>
-    <row r="52" spans="1:35" ht="24" customHeight="1">
+    <row r="52" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="48"/>
@@ -3635,7 +3641,7 @@
       </c>
       <c r="AI52" s="96"/>
     </row>
-    <row r="53" spans="1:35" ht="24" customHeight="1">
+    <row r="53" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="48"/>
@@ -3675,7 +3681,7 @@
       </c>
       <c r="AI53" s="96"/>
     </row>
-    <row r="54" spans="1:35" ht="24" customHeight="1">
+    <row r="54" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="48"/>
@@ -3715,7 +3721,7 @@
       </c>
       <c r="AI54" s="96"/>
     </row>
-    <row r="55" spans="1:35" ht="24" customHeight="1">
+    <row r="55" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="48"/>
@@ -3755,7 +3761,7 @@
       </c>
       <c r="AI55" s="96"/>
     </row>
-    <row r="56" spans="1:35" ht="24" customHeight="1">
+    <row r="56" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="48"/>
@@ -3795,7 +3801,7 @@
       </c>
       <c r="AI56" s="96"/>
     </row>
-    <row r="57" spans="1:35" ht="24" customHeight="1">
+    <row r="57" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="48"/>
@@ -3835,7 +3841,7 @@
       </c>
       <c r="AI57" s="96"/>
     </row>
-    <row r="58" spans="1:35" ht="24" customHeight="1">
+    <row r="58" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="48"/>
@@ -3875,7 +3881,7 @@
       </c>
       <c r="AI58" s="96"/>
     </row>
-    <row r="59" spans="1:35" ht="24" customHeight="1">
+    <row r="59" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="13"/>
       <c r="B59" s="51"/>
       <c r="C59" s="48"/>
@@ -3915,7 +3921,7 @@
       </c>
       <c r="AI59" s="96"/>
     </row>
-    <row r="60" spans="1:35" ht="24" customHeight="1">
+    <row r="60" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="13"/>
       <c r="B60" s="51"/>
       <c r="C60" s="48"/>
@@ -3955,7 +3961,7 @@
       </c>
       <c r="AI60" s="96"/>
     </row>
-    <row r="61" spans="1:35" ht="24" customHeight="1">
+    <row r="61" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="13"/>
       <c r="B61" s="51"/>
       <c r="C61" s="48"/>
@@ -3995,7 +4001,7 @@
       </c>
       <c r="AI61" s="96"/>
     </row>
-    <row r="62" spans="1:35" ht="24" customHeight="1">
+    <row r="62" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="13"/>
       <c r="B62" s="51"/>
       <c r="C62" s="48"/>
@@ -4035,7 +4041,7 @@
       </c>
       <c r="AI62" s="96"/>
     </row>
-    <row r="63" spans="1:35" ht="24" customHeight="1">
+    <row r="63" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="13"/>
       <c r="B63" s="51"/>
       <c r="C63" s="48"/>
@@ -4075,7 +4081,7 @@
       </c>
       <c r="AI63" s="96"/>
     </row>
-    <row r="64" spans="1:35" ht="24" customHeight="1">
+    <row r="64" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="13"/>
       <c r="B64" s="51"/>
       <c r="C64" s="48"/>
@@ -4115,7 +4121,7 @@
       </c>
       <c r="AI64" s="96"/>
     </row>
-    <row r="65" spans="1:35" ht="24" customHeight="1">
+    <row r="65" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="13"/>
       <c r="B65" s="51"/>
       <c r="C65" s="48"/>
@@ -4155,7 +4161,7 @@
       </c>
       <c r="AI65" s="96"/>
     </row>
-    <row r="66" spans="1:35" ht="24" customHeight="1">
+    <row r="66" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="13"/>
       <c r="B66" s="51"/>
       <c r="C66" s="48"/>
@@ -4195,7 +4201,7 @@
       </c>
       <c r="AI66" s="96"/>
     </row>
-    <row r="67" spans="1:35" ht="24" customHeight="1">
+    <row r="67" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="13"/>
       <c r="B67" s="51"/>
       <c r="C67" s="48"/>
@@ -4235,7 +4241,7 @@
       </c>
       <c r="AI67" s="96"/>
     </row>
-    <row r="68" spans="1:35" ht="24" customHeight="1">
+    <row r="68" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="46"/>
       <c r="B68" s="46"/>
       <c r="C68" s="48"/>
@@ -4275,7 +4281,7 @@
       </c>
       <c r="AI68" s="96"/>
     </row>
-    <row r="69" spans="1:35" ht="24" customHeight="1">
+    <row r="69" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="46"/>
       <c r="B69" s="46"/>
       <c r="C69" s="48"/>
@@ -4315,7 +4321,7 @@
       </c>
       <c r="AI69" s="96"/>
     </row>
-    <row r="70" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="70" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="52" t="s">
         <v>19</v>
       </c>
@@ -4357,7 +4363,7 @@
       </c>
       <c r="AI70" s="96"/>
     </row>
-    <row r="71" spans="1:35" ht="24" customHeight="1">
+    <row r="71" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="42" t="s">
         <v>21</v>
       </c>
@@ -4403,7 +4409,7 @@
       </c>
       <c r="AI71" s="96"/>
     </row>
-    <row r="72" spans="1:35" ht="24" customHeight="1">
+    <row r="72" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="42" t="s">
         <v>22</v>
       </c>
@@ -4449,7 +4455,7 @@
       </c>
       <c r="AI72" s="96"/>
     </row>
-    <row r="73" spans="1:35" ht="24" customHeight="1">
+    <row r="73" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="42" t="s">
         <v>23</v>
       </c>
@@ -4497,7 +4503,7 @@
       </c>
       <c r="AI73" s="96"/>
     </row>
-    <row r="74" spans="1:35" ht="24" customHeight="1">
+    <row r="74" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="87"/>
       <c r="B74" s="32"/>
       <c r="C74" s="48"/>
@@ -4541,7 +4547,7 @@
       </c>
       <c r="AI74" s="96"/>
     </row>
-    <row r="75" spans="1:35" ht="24" customHeight="1">
+    <row r="75" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="49"/>
       <c r="B75" s="50"/>
       <c r="C75" s="48"/>
@@ -4581,7 +4587,7 @@
       </c>
       <c r="AI75" s="96"/>
     </row>
-    <row r="76" spans="1:35" ht="24" customHeight="1">
+    <row r="76" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="45"/>
       <c r="B76" s="50"/>
       <c r="C76" s="48"/>
@@ -4621,7 +4627,7 @@
       </c>
       <c r="AI76" s="96"/>
     </row>
-    <row r="77" spans="1:35" ht="15">
+    <row r="77" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="70"/>
       <c r="B77" s="50"/>
       <c r="C77" s="48"/>
@@ -4661,7 +4667,7 @@
       </c>
       <c r="AI77" s="96"/>
     </row>
-    <row r="78" spans="1:35" ht="24" customHeight="1">
+    <row r="78" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="70"/>
       <c r="B78" s="50"/>
       <c r="C78" s="48"/>
@@ -4701,7 +4707,7 @@
       </c>
       <c r="AI78" s="96"/>
     </row>
-    <row r="79" spans="1:35" ht="24" customHeight="1">
+    <row r="79" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="87"/>
       <c r="B79" s="50"/>
       <c r="C79" s="48"/>
@@ -4741,7 +4747,7 @@
       </c>
       <c r="AI79" s="96"/>
     </row>
-    <row r="80" spans="1:35" ht="24" customHeight="1">
+    <row r="80" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="70"/>
       <c r="B80" s="50"/>
       <c r="C80" s="48"/>
@@ -4781,7 +4787,7 @@
       </c>
       <c r="AI80" s="96"/>
     </row>
-    <row r="81" spans="1:35" ht="24" customHeight="1">
+    <row r="81" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="70"/>
       <c r="B81" s="50"/>
       <c r="C81" s="48"/>
@@ -4821,7 +4827,7 @@
       </c>
       <c r="AI81" s="96"/>
     </row>
-    <row r="82" spans="1:35" ht="24" customHeight="1">
+    <row r="82" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="42"/>
       <c r="B82" s="50"/>
       <c r="C82" s="48"/>
@@ -4861,7 +4867,7 @@
       </c>
       <c r="AI82" s="96"/>
     </row>
-    <row r="83" spans="1:35" ht="24" customHeight="1">
+    <row r="83" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="42"/>
       <c r="B83" s="50"/>
       <c r="C83" s="48"/>
@@ -4901,7 +4907,7 @@
       </c>
       <c r="AI83" s="96"/>
     </row>
-    <row r="84" spans="1:35" ht="24" customHeight="1">
+    <row r="84" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="42"/>
       <c r="B84" s="50"/>
       <c r="C84" s="48"/>
@@ -4941,7 +4947,7 @@
       </c>
       <c r="AI84" s="96"/>
     </row>
-    <row r="85" spans="1:35" ht="24" customHeight="1">
+    <row r="85" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="42"/>
       <c r="B85" s="50"/>
       <c r="C85" s="48"/>
@@ -4981,7 +4987,7 @@
       </c>
       <c r="AI85" s="96"/>
     </row>
-    <row r="86" spans="1:35" ht="24" customHeight="1">
+    <row r="86" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="42"/>
       <c r="B86" s="50"/>
       <c r="C86" s="48"/>
@@ -5021,7 +5027,7 @@
       </c>
       <c r="AI86" s="96"/>
     </row>
-    <row r="87" spans="1:35" ht="27" customHeight="1">
+    <row r="87" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="42"/>
       <c r="B87" s="50"/>
       <c r="C87" s="48"/>
@@ -5061,7 +5067,7 @@
       </c>
       <c r="AI87" s="96"/>
     </row>
-    <row r="88" spans="1:35" ht="24" customHeight="1">
+    <row r="88" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="70"/>
       <c r="B88" s="50"/>
       <c r="C88" s="48"/>
@@ -5101,7 +5107,7 @@
       </c>
       <c r="AI88" s="96"/>
     </row>
-    <row r="89" spans="1:35" ht="24" customHeight="1">
+    <row r="89" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="70"/>
       <c r="B89" s="50"/>
       <c r="C89" s="48"/>
@@ -5141,7 +5147,7 @@
       </c>
       <c r="AI89" s="96"/>
     </row>
-    <row r="90" spans="1:35" ht="24" customHeight="1">
+    <row r="90" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="70"/>
       <c r="B90" s="50"/>
       <c r="C90" s="48"/>
@@ -5181,7 +5187,7 @@
       </c>
       <c r="AI90" s="96"/>
     </row>
-    <row r="91" spans="1:35" ht="24" customHeight="1">
+    <row r="91" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="56"/>
       <c r="B91" s="32"/>
       <c r="C91" s="48"/>
@@ -5221,7 +5227,7 @@
       </c>
       <c r="AI91" s="96"/>
     </row>
-    <row r="92" spans="1:35" ht="24" customHeight="1">
+    <row r="92" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="13"/>
       <c r="B92" s="32"/>
       <c r="C92" s="48"/>
@@ -5261,7 +5267,7 @@
       </c>
       <c r="AI92" s="96"/>
     </row>
-    <row r="93" spans="1:35" ht="24" customHeight="1">
+    <row r="93" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="13"/>
       <c r="B93" s="32"/>
       <c r="C93" s="48"/>
@@ -5301,7 +5307,7 @@
       </c>
       <c r="AI93" s="96"/>
     </row>
-    <row r="94" spans="1:35" ht="24" customHeight="1">
+    <row r="94" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="13"/>
       <c r="B94" s="32"/>
       <c r="C94" s="48"/>
@@ -5341,7 +5347,7 @@
       </c>
       <c r="AI94" s="96"/>
     </row>
-    <row r="95" spans="1:35" ht="24" customHeight="1">
+    <row r="95" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="13"/>
       <c r="B95" s="32"/>
       <c r="C95" s="48"/>
@@ -5381,7 +5387,7 @@
       </c>
       <c r="AI95" s="96"/>
     </row>
-    <row r="96" spans="1:35" ht="24" customHeight="1">
+    <row r="96" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="13"/>
       <c r="B96" s="32"/>
       <c r="C96" s="48"/>
@@ -5421,7 +5427,7 @@
       </c>
       <c r="AI96" s="96"/>
     </row>
-    <row r="97" spans="1:35" ht="24" customHeight="1">
+    <row r="97" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="13"/>
       <c r="B97" s="32"/>
       <c r="C97" s="48"/>
@@ -5461,7 +5467,7 @@
       </c>
       <c r="AI97" s="96"/>
     </row>
-    <row r="98" spans="1:35" ht="24" customHeight="1">
+    <row r="98" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="13"/>
       <c r="B98" s="32"/>
       <c r="C98" s="48"/>
@@ -5501,7 +5507,7 @@
       </c>
       <c r="AI98" s="96"/>
     </row>
-    <row r="99" spans="1:35" ht="24" customHeight="1">
+    <row r="99" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="13"/>
       <c r="B99" s="32"/>
       <c r="C99" s="48"/>
@@ -5541,7 +5547,7 @@
       </c>
       <c r="AI99" s="97"/>
     </row>
-    <row r="100" spans="1:35" ht="37.5" customHeight="1">
+    <row r="100" spans="1:35" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
         <v>0</v>
       </c>
@@ -5679,7 +5685,7 @@
         <v>22.727272727272727</v>
       </c>
     </row>
-    <row r="101" spans="1:35">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A101" s="14"/>
       <c r="B101" s="15"/>
     </row>
@@ -5766,7 +5772,7 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6:B74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="49" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
@@ -5778,7 +5784,7 @@
     <col min="36" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="35.25" customHeight="1">
+    <row r="1" spans="1:35" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>4</v>
       </c>
@@ -5818,7 +5824,7 @@
       <c r="AG1" s="90"/>
       <c r="AH1" s="90"/>
     </row>
-    <row r="2" spans="1:35" ht="24.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:35" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="23"/>
@@ -5855,7 +5861,7 @@
       <c r="AH2" s="25"/>
       <c r="AI2" s="25"/>
     </row>
-    <row r="3" spans="1:35" ht="15.75" thickBot="1">
+    <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
@@ -5894,7 +5900,7 @@
       <c r="AH3" s="94"/>
       <c r="AI3" s="57"/>
     </row>
-    <row r="4" spans="1:35" ht="36.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:35" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>42767</v>
       </c>
@@ -5938,7 +5944,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="25.5" thickBot="1">
+    <row r="5" spans="1:35" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="61" t="s">
         <v>5</v>
       </c>
@@ -6067,7 +6073,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="23.45" customHeight="1" thickBot="1">
+    <row r="6" spans="1:35" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>14</v>
       </c>
@@ -6190,7 +6196,7 @@
       <c r="AH6" s="59"/>
       <c r="AI6" s="59"/>
     </row>
-    <row r="7" spans="1:35" ht="23.45" customHeight="1">
+    <row r="7" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
         <v>9</v>
       </c>
@@ -6232,7 +6238,7 @@
       </c>
       <c r="AI7" s="98"/>
     </row>
-    <row r="8" spans="1:35" ht="23.45" customHeight="1">
+    <row r="8" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
@@ -6274,7 +6280,7 @@
       </c>
       <c r="AI8" s="96"/>
     </row>
-    <row r="9" spans="1:35" ht="23.45" customHeight="1">
+    <row r="9" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="32"/>
       <c r="C9" s="47"/>
@@ -6314,7 +6320,7 @@
       </c>
       <c r="AI9" s="96"/>
     </row>
-    <row r="10" spans="1:35" ht="23.45" customHeight="1">
+    <row r="10" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="32"/>
       <c r="C10" s="47"/>
@@ -6354,7 +6360,7 @@
       </c>
       <c r="AI10" s="96"/>
     </row>
-    <row r="11" spans="1:35" ht="23.45" customHeight="1">
+    <row r="11" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
       <c r="B11" s="32"/>
       <c r="C11" s="47"/>
@@ -6394,7 +6400,7 @@
       </c>
       <c r="AI11" s="96"/>
     </row>
-    <row r="12" spans="1:35" ht="23.45" customHeight="1">
+    <row r="12" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="51"/>
       <c r="C12" s="47"/>
@@ -6434,7 +6440,7 @@
       </c>
       <c r="AI12" s="96"/>
     </row>
-    <row r="13" spans="1:35" ht="23.45" customHeight="1" thickBot="1">
+    <row r="13" spans="1:35" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
         <v>11</v>
       </c>
@@ -6476,7 +6482,7 @@
       </c>
       <c r="AI13" s="96"/>
     </row>
-    <row r="14" spans="1:35" ht="23.45" customHeight="1">
+    <row r="14" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
         <v>13</v>
       </c>
@@ -6518,7 +6524,7 @@
       </c>
       <c r="AI14" s="96"/>
     </row>
-    <row r="15" spans="1:35" ht="23.45" customHeight="1">
+    <row r="15" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
         <v>12</v>
       </c>
@@ -6560,7 +6566,7 @@
       </c>
       <c r="AI15" s="96"/>
     </row>
-    <row r="16" spans="1:35" ht="23.45" customHeight="1">
+    <row r="16" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="32"/>
       <c r="C16" s="47"/>
@@ -6600,7 +6606,7 @@
       </c>
       <c r="AI16" s="96"/>
     </row>
-    <row r="17" spans="1:35" ht="23.45" customHeight="1">
+    <row r="17" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="32"/>
       <c r="C17" s="47"/>
@@ -6640,7 +6646,7 @@
       </c>
       <c r="AI17" s="96"/>
     </row>
-    <row r="18" spans="1:35" ht="22.9" customHeight="1">
+    <row r="18" spans="1:35" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="32"/>
       <c r="C18" s="47"/>
@@ -6680,7 +6686,7 @@
       </c>
       <c r="AI18" s="96"/>
     </row>
-    <row r="19" spans="1:35" ht="23.45" customHeight="1">
+    <row r="19" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="32"/>
       <c r="C19" s="47"/>
@@ -6720,7 +6726,7 @@
       </c>
       <c r="AI19" s="96"/>
     </row>
-    <row r="20" spans="1:35" ht="23.45" customHeight="1">
+    <row r="20" spans="1:35" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="51"/>
       <c r="C20" s="47"/>
@@ -6760,7 +6766,7 @@
       </c>
       <c r="AI20" s="96"/>
     </row>
-    <row r="21" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="21" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
         <v>15</v>
       </c>
@@ -6802,7 +6808,7 @@
       </c>
       <c r="AI21" s="96"/>
     </row>
-    <row r="22" spans="1:35" ht="24" customHeight="1">
+    <row r="22" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>16</v>
       </c>
@@ -6846,7 +6852,7 @@
       </c>
       <c r="AI22" s="96"/>
     </row>
-    <row r="23" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="23" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="43" t="s">
         <v>10</v>
@@ -6888,7 +6894,7 @@
       </c>
       <c r="AI23" s="96"/>
     </row>
-    <row r="24" spans="1:35" ht="24" customHeight="1">
+    <row r="24" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>17</v>
       </c>
@@ -6932,7 +6938,7 @@
       </c>
       <c r="AI24" s="96"/>
     </row>
-    <row r="25" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="25" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
       <c r="B25" s="43" t="s">
         <v>10</v>
@@ -6974,7 +6980,7 @@
       </c>
       <c r="AI25" s="96"/>
     </row>
-    <row r="26" spans="1:35" ht="24" customHeight="1">
+    <row r="26" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
         <v>18</v>
       </c>
@@ -7018,7 +7024,7 @@
       </c>
       <c r="AI26" s="96"/>
     </row>
-    <row r="27" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="27" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27" s="43" t="s">
         <v>10</v>
@@ -7060,7 +7066,7 @@
       </c>
       <c r="AI27" s="96"/>
     </row>
-    <row r="28" spans="1:35" ht="24" customHeight="1">
+    <row r="28" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="30"/>
       <c r="B28" s="44"/>
       <c r="C28" s="47"/>
@@ -7100,7 +7106,7 @@
       </c>
       <c r="AI28" s="96"/>
     </row>
-    <row r="29" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="29" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
       <c r="B29" s="43"/>
       <c r="C29" s="47"/>
@@ -7140,7 +7146,7 @@
       </c>
       <c r="AI29" s="96"/>
     </row>
-    <row r="30" spans="1:35" ht="24" customHeight="1">
+    <row r="30" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30"/>
       <c r="B30" s="44"/>
       <c r="C30" s="47"/>
@@ -7180,7 +7186,7 @@
       </c>
       <c r="AI30" s="96"/>
     </row>
-    <row r="31" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="31" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="B31" s="43"/>
       <c r="C31" s="47"/>
@@ -7220,7 +7226,7 @@
       </c>
       <c r="AI31" s="96"/>
     </row>
-    <row r="32" spans="1:35" ht="24" customHeight="1">
+    <row r="32" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="45"/>
       <c r="B32" s="44"/>
       <c r="C32" s="47"/>
@@ -7260,7 +7266,7 @@
       </c>
       <c r="AI32" s="96"/>
     </row>
-    <row r="33" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="33" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
       <c r="B33" s="43"/>
       <c r="C33" s="47"/>
@@ -7300,7 +7306,7 @@
       </c>
       <c r="AI33" s="96"/>
     </row>
-    <row r="34" spans="1:35" ht="24" customHeight="1">
+    <row r="34" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="45"/>
       <c r="B34" s="44"/>
       <c r="C34" s="47"/>
@@ -7340,7 +7346,7 @@
       </c>
       <c r="AI34" s="96"/>
     </row>
-    <row r="35" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="35" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
       <c r="B35" s="53"/>
       <c r="C35" s="47"/>
@@ -7380,7 +7386,7 @@
       </c>
       <c r="AI35" s="96"/>
     </row>
-    <row r="36" spans="1:35" ht="24" customHeight="1">
+    <row r="36" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="49"/>
       <c r="B36" s="44"/>
       <c r="C36" s="47"/>
@@ -7420,7 +7426,7 @@
       </c>
       <c r="AI36" s="96"/>
     </row>
-    <row r="37" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="37" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="B37" s="53"/>
       <c r="C37" s="47"/>
@@ -7460,7 +7466,7 @@
       </c>
       <c r="AI37" s="96"/>
     </row>
-    <row r="38" spans="1:35" ht="24" customHeight="1">
+    <row r="38" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="45"/>
       <c r="B38" s="44"/>
       <c r="C38" s="47"/>
@@ -7500,7 +7506,7 @@
       </c>
       <c r="AI38" s="96"/>
     </row>
-    <row r="39" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="39" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="53"/>
       <c r="C39" s="47"/>
@@ -7540,7 +7546,7 @@
       </c>
       <c r="AI39" s="96"/>
     </row>
-    <row r="40" spans="1:35" ht="24" customHeight="1">
+    <row r="40" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="13"/>
       <c r="B40" s="44"/>
       <c r="C40" s="47"/>
@@ -7580,7 +7586,7 @@
       </c>
       <c r="AI40" s="96"/>
     </row>
-    <row r="41" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="41" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31"/>
       <c r="B41" s="53"/>
       <c r="C41" s="47"/>
@@ -7620,7 +7626,7 @@
       </c>
       <c r="AI41" s="96"/>
     </row>
-    <row r="42" spans="1:35" ht="24" customHeight="1">
+    <row r="42" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13"/>
       <c r="B42" s="44"/>
       <c r="C42" s="47"/>
@@ -7660,7 +7666,7 @@
       </c>
       <c r="AI42" s="96"/>
     </row>
-    <row r="43" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="43" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31"/>
       <c r="B43" s="43"/>
       <c r="C43" s="47"/>
@@ -7700,7 +7706,7 @@
       </c>
       <c r="AI43" s="96"/>
     </row>
-    <row r="44" spans="1:35" ht="24" customHeight="1">
+    <row r="44" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="30"/>
       <c r="B44" s="44"/>
       <c r="C44" s="47"/>
@@ -7740,7 +7746,7 @@
       </c>
       <c r="AI44" s="96"/>
     </row>
-    <row r="45" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="45" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="43"/>
       <c r="C45" s="47"/>
@@ -7780,7 +7786,7 @@
       </c>
       <c r="AI45" s="96"/>
     </row>
-    <row r="46" spans="1:35" ht="24" customHeight="1">
+    <row r="46" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="49"/>
       <c r="B46" s="44"/>
       <c r="C46" s="47"/>
@@ -7820,7 +7826,7 @@
       </c>
       <c r="AI46" s="96"/>
     </row>
-    <row r="47" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="47" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="43"/>
       <c r="C47" s="47"/>
@@ -7860,7 +7866,7 @@
       </c>
       <c r="AI47" s="96"/>
     </row>
-    <row r="48" spans="1:35" ht="24" customHeight="1">
+    <row r="48" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="42"/>
       <c r="B48" s="44"/>
       <c r="C48" s="47"/>
@@ -7900,7 +7906,7 @@
       </c>
       <c r="AI48" s="96"/>
     </row>
-    <row r="49" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="49" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="43"/>
       <c r="C49" s="47"/>
@@ -7940,7 +7946,7 @@
       </c>
       <c r="AI49" s="96"/>
     </row>
-    <row r="50" spans="1:35" ht="24" customHeight="1">
+    <row r="50" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
       <c r="B50" s="30"/>
       <c r="C50" s="47"/>
@@ -7980,7 +7986,7 @@
       </c>
       <c r="AI50" s="96"/>
     </row>
-    <row r="51" spans="1:35" ht="24" customHeight="1">
+    <row r="51" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="47"/>
@@ -8020,7 +8026,7 @@
       </c>
       <c r="AI51" s="96"/>
     </row>
-    <row r="52" spans="1:35" ht="24" customHeight="1">
+    <row r="52" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="47"/>
@@ -8060,7 +8066,7 @@
       </c>
       <c r="AI52" s="96"/>
     </row>
-    <row r="53" spans="1:35" ht="24" customHeight="1">
+    <row r="53" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="47"/>
@@ -8100,7 +8106,7 @@
       </c>
       <c r="AI53" s="96"/>
     </row>
-    <row r="54" spans="1:35" ht="24" customHeight="1">
+    <row r="54" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="47"/>
@@ -8140,7 +8146,7 @@
       </c>
       <c r="AI54" s="96"/>
     </row>
-    <row r="55" spans="1:35" ht="24" customHeight="1">
+    <row r="55" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="47"/>
@@ -8180,7 +8186,7 @@
       </c>
       <c r="AI55" s="96"/>
     </row>
-    <row r="56" spans="1:35" ht="24" customHeight="1">
+    <row r="56" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="47"/>
@@ -8220,7 +8226,7 @@
       </c>
       <c r="AI56" s="96"/>
     </row>
-    <row r="57" spans="1:35" ht="24" customHeight="1">
+    <row r="57" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="47"/>
@@ -8260,7 +8266,7 @@
       </c>
       <c r="AI57" s="96"/>
     </row>
-    <row r="58" spans="1:35" ht="24" customHeight="1">
+    <row r="58" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="47"/>
@@ -8300,7 +8306,7 @@
       </c>
       <c r="AI58" s="96"/>
     </row>
-    <row r="59" spans="1:35" ht="24" customHeight="1">
+    <row r="59" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="13"/>
       <c r="B59" s="51"/>
       <c r="C59" s="47"/>
@@ -8340,7 +8346,7 @@
       </c>
       <c r="AI59" s="96"/>
     </row>
-    <row r="60" spans="1:35" ht="24" customHeight="1">
+    <row r="60" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="13"/>
       <c r="B60" s="51"/>
       <c r="C60" s="47"/>
@@ -8380,7 +8386,7 @@
       </c>
       <c r="AI60" s="96"/>
     </row>
-    <row r="61" spans="1:35" ht="24" customHeight="1">
+    <row r="61" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="13"/>
       <c r="B61" s="51"/>
       <c r="C61" s="47"/>
@@ -8420,7 +8426,7 @@
       </c>
       <c r="AI61" s="96"/>
     </row>
-    <row r="62" spans="1:35" ht="24" customHeight="1">
+    <row r="62" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="13"/>
       <c r="B62" s="51"/>
       <c r="C62" s="47"/>
@@ -8460,7 +8466,7 @@
       </c>
       <c r="AI62" s="96"/>
     </row>
-    <row r="63" spans="1:35" ht="24" customHeight="1">
+    <row r="63" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="13"/>
       <c r="B63" s="51"/>
       <c r="C63" s="47"/>
@@ -8500,7 +8506,7 @@
       </c>
       <c r="AI63" s="96"/>
     </row>
-    <row r="64" spans="1:35" ht="24" customHeight="1">
+    <row r="64" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="13"/>
       <c r="B64" s="51"/>
       <c r="C64" s="47"/>
@@ -8540,7 +8546,7 @@
       </c>
       <c r="AI64" s="96"/>
     </row>
-    <row r="65" spans="1:35" ht="24" customHeight="1">
+    <row r="65" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="13"/>
       <c r="B65" s="51"/>
       <c r="C65" s="47"/>
@@ -8580,7 +8586,7 @@
       </c>
       <c r="AI65" s="96"/>
     </row>
-    <row r="66" spans="1:35" ht="24" customHeight="1">
+    <row r="66" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="13"/>
       <c r="B66" s="51"/>
       <c r="C66" s="47"/>
@@ -8620,7 +8626,7 @@
       </c>
       <c r="AI66" s="96"/>
     </row>
-    <row r="67" spans="1:35" ht="24" customHeight="1">
+    <row r="67" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="13"/>
       <c r="B67" s="51"/>
       <c r="C67" s="47"/>
@@ -8660,7 +8666,7 @@
       </c>
       <c r="AI67" s="96"/>
     </row>
-    <row r="68" spans="1:35" ht="24" customHeight="1">
+    <row r="68" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="46"/>
       <c r="B68" s="46"/>
       <c r="C68" s="47"/>
@@ -8700,7 +8706,7 @@
       </c>
       <c r="AI68" s="96"/>
     </row>
-    <row r="69" spans="1:35" ht="24" customHeight="1">
+    <row r="69" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="46"/>
       <c r="B69" s="46"/>
       <c r="C69" s="47"/>
@@ -8740,7 +8746,7 @@
       </c>
       <c r="AI69" s="96"/>
     </row>
-    <row r="70" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="70" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="52" t="s">
         <v>19</v>
       </c>
@@ -8782,7 +8788,7 @@
       </c>
       <c r="AI70" s="96"/>
     </row>
-    <row r="71" spans="1:35" ht="24" customHeight="1">
+    <row r="71" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="42" t="s">
         <v>21</v>
       </c>
@@ -8826,7 +8832,7 @@
       </c>
       <c r="AI71" s="96"/>
     </row>
-    <row r="72" spans="1:35" ht="24" customHeight="1">
+    <row r="72" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="42" t="s">
         <v>22</v>
       </c>
@@ -8870,7 +8876,7 @@
       </c>
       <c r="AI72" s="96"/>
     </row>
-    <row r="73" spans="1:35" ht="24" customHeight="1">
+    <row r="73" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="42" t="s">
         <v>23</v>
       </c>
@@ -8914,7 +8920,7 @@
       </c>
       <c r="AI73" s="96"/>
     </row>
-    <row r="74" spans="1:35" ht="24" customHeight="1">
+    <row r="74" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="87"/>
       <c r="B74" s="32"/>
       <c r="C74" s="47"/>
@@ -8954,7 +8960,7 @@
       </c>
       <c r="AI74" s="96"/>
     </row>
-    <row r="75" spans="1:35" ht="24" customHeight="1">
+    <row r="75" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="49"/>
       <c r="B75" s="50"/>
       <c r="C75" s="47"/>
@@ -8994,7 +9000,7 @@
       </c>
       <c r="AI75" s="96"/>
     </row>
-    <row r="76" spans="1:35" ht="24" customHeight="1">
+    <row r="76" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="45"/>
       <c r="B76" s="50"/>
       <c r="C76" s="47"/>
@@ -9034,7 +9040,7 @@
       </c>
       <c r="AI76" s="96"/>
     </row>
-    <row r="77" spans="1:35" ht="24" customHeight="1">
+    <row r="77" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="70"/>
       <c r="B77" s="50"/>
       <c r="C77" s="47"/>
@@ -9074,7 +9080,7 @@
       </c>
       <c r="AI77" s="96"/>
     </row>
-    <row r="78" spans="1:35" ht="24" customHeight="1">
+    <row r="78" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="70"/>
       <c r="B78" s="50"/>
       <c r="C78" s="47"/>
@@ -9114,7 +9120,7 @@
       </c>
       <c r="AI78" s="96"/>
     </row>
-    <row r="79" spans="1:35" ht="24" customHeight="1">
+    <row r="79" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="87"/>
       <c r="B79" s="50"/>
       <c r="C79" s="47"/>
@@ -9154,7 +9160,7 @@
       </c>
       <c r="AI79" s="96"/>
     </row>
-    <row r="80" spans="1:35" ht="24" customHeight="1">
+    <row r="80" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="70"/>
       <c r="B80" s="50"/>
       <c r="C80" s="47"/>
@@ -9194,7 +9200,7 @@
       </c>
       <c r="AI80" s="96"/>
     </row>
-    <row r="81" spans="1:35" ht="24" customHeight="1">
+    <row r="81" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="70"/>
       <c r="B81" s="50"/>
       <c r="C81" s="47"/>
@@ -9234,7 +9240,7 @@
       </c>
       <c r="AI81" s="96"/>
     </row>
-    <row r="82" spans="1:35" ht="24" customHeight="1">
+    <row r="82" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="42"/>
       <c r="B82" s="50"/>
       <c r="C82" s="47"/>
@@ -9274,7 +9280,7 @@
       </c>
       <c r="AI82" s="96"/>
     </row>
-    <row r="83" spans="1:35" ht="24" customHeight="1">
+    <row r="83" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="42"/>
       <c r="B83" s="50"/>
       <c r="C83" s="47"/>
@@ -9314,7 +9320,7 @@
       </c>
       <c r="AI83" s="96"/>
     </row>
-    <row r="84" spans="1:35" ht="24" customHeight="1">
+    <row r="84" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="70"/>
       <c r="B84" s="50"/>
       <c r="C84" s="47"/>
@@ -9354,7 +9360,7 @@
       </c>
       <c r="AI84" s="96"/>
     </row>
-    <row r="85" spans="1:35" ht="24" customHeight="1">
+    <row r="85" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="70"/>
       <c r="B85" s="50"/>
       <c r="C85" s="47"/>
@@ -9394,7 +9400,7 @@
       </c>
       <c r="AI85" s="96"/>
     </row>
-    <row r="86" spans="1:35" ht="24" customHeight="1">
+    <row r="86" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="70"/>
       <c r="B86" s="50"/>
       <c r="C86" s="47"/>
@@ -9434,7 +9440,7 @@
       </c>
       <c r="AI86" s="96"/>
     </row>
-    <row r="87" spans="1:35" ht="45.75" customHeight="1">
+    <row r="87" spans="1:35" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="70"/>
       <c r="B87" s="50"/>
       <c r="C87" s="47"/>
@@ -9474,7 +9480,7 @@
       </c>
       <c r="AI87" s="96"/>
     </row>
-    <row r="88" spans="1:35" ht="24" customHeight="1">
+    <row r="88" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="70"/>
       <c r="B88" s="50"/>
       <c r="C88" s="47"/>
@@ -9514,7 +9520,7 @@
       </c>
       <c r="AI88" s="96"/>
     </row>
-    <row r="89" spans="1:35" ht="24" customHeight="1">
+    <row r="89" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="70"/>
       <c r="B89" s="50"/>
       <c r="C89" s="47"/>
@@ -9554,7 +9560,7 @@
       </c>
       <c r="AI89" s="96"/>
     </row>
-    <row r="90" spans="1:35" ht="24" customHeight="1">
+    <row r="90" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="70"/>
       <c r="B90" s="50"/>
       <c r="C90" s="47"/>
@@ -9594,7 +9600,7 @@
       </c>
       <c r="AI90" s="96"/>
     </row>
-    <row r="91" spans="1:35" ht="24" customHeight="1">
+    <row r="91" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="70"/>
       <c r="B91" s="50"/>
       <c r="C91" s="47"/>
@@ -9634,7 +9640,7 @@
       </c>
       <c r="AI91" s="96"/>
     </row>
-    <row r="92" spans="1:35" ht="24" customHeight="1">
+    <row r="92" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="13"/>
       <c r="B92" s="51"/>
       <c r="C92" s="47"/>
@@ -9674,7 +9680,7 @@
       </c>
       <c r="AI92" s="96"/>
     </row>
-    <row r="93" spans="1:35" ht="24" customHeight="1">
+    <row r="93" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="13"/>
       <c r="B93" s="51"/>
       <c r="C93" s="47"/>
@@ -9714,7 +9720,7 @@
       </c>
       <c r="AI93" s="96"/>
     </row>
-    <row r="94" spans="1:35" ht="24" customHeight="1">
+    <row r="94" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="13"/>
       <c r="B94" s="51"/>
       <c r="C94" s="47"/>
@@ -9754,7 +9760,7 @@
       </c>
       <c r="AI94" s="96"/>
     </row>
-    <row r="95" spans="1:35" ht="24" customHeight="1">
+    <row r="95" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="13"/>
       <c r="B95" s="51"/>
       <c r="C95" s="47"/>
@@ -9794,7 +9800,7 @@
       </c>
       <c r="AI95" s="96"/>
     </row>
-    <row r="96" spans="1:35" ht="24" customHeight="1">
+    <row r="96" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="13"/>
       <c r="B96" s="51"/>
       <c r="C96" s="47"/>
@@ -9834,7 +9840,7 @@
       </c>
       <c r="AI96" s="96"/>
     </row>
-    <row r="97" spans="1:35" ht="24" customHeight="1">
+    <row r="97" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="13"/>
       <c r="B97" s="51"/>
       <c r="C97" s="47"/>
@@ -9874,7 +9880,7 @@
       </c>
       <c r="AI97" s="96"/>
     </row>
-    <row r="98" spans="1:35" ht="24" customHeight="1">
+    <row r="98" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="13"/>
       <c r="B98" s="51"/>
       <c r="C98" s="47"/>
@@ -9914,7 +9920,7 @@
       </c>
       <c r="AI98" s="96"/>
     </row>
-    <row r="99" spans="1:35" ht="24" customHeight="1">
+    <row r="99" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="13"/>
       <c r="B99" s="51"/>
       <c r="C99" s="47"/>
@@ -9954,7 +9960,7 @@
       </c>
       <c r="AI99" s="97"/>
     </row>
-    <row r="100" spans="1:35" ht="37.5" customHeight="1">
+    <row r="100" spans="1:35" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
         <v>0</v>
       </c>
@@ -10089,7 +10095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:35">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A101" s="14"/>
       <c r="B101" s="15"/>
     </row>
@@ -10141,7 +10147,7 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6:B74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -10156,7 +10162,7 @@
     <col min="36" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="35.25" customHeight="1">
+    <row r="1" spans="1:35" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>4</v>
       </c>
@@ -10196,7 +10202,7 @@
       <c r="AG1" s="90"/>
       <c r="AH1" s="90"/>
     </row>
-    <row r="2" spans="1:35" ht="24.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:35" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="23"/>
@@ -10233,7 +10239,7 @@
       <c r="AH2" s="25"/>
       <c r="AI2" s="25"/>
     </row>
-    <row r="3" spans="1:35" ht="15.75" thickBot="1">
+    <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
@@ -10272,7 +10278,7 @@
       <c r="AH3" s="94"/>
       <c r="AI3" s="57"/>
     </row>
-    <row r="4" spans="1:35" ht="36.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:35" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="62">
         <v>42795</v>
       </c>
@@ -10316,7 +10322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="18.75" thickBot="1">
+    <row r="5" spans="1:35" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="61" t="s">
         <v>5</v>
       </c>
@@ -10454,7 +10460,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="20.25" customHeight="1" thickBot="1">
+    <row r="6" spans="1:35" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>14</v>
       </c>
@@ -10586,7 +10592,7 @@
       <c r="AH6" s="59"/>
       <c r="AI6" s="59"/>
     </row>
-    <row r="7" spans="1:35" ht="24" customHeight="1">
+    <row r="7" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
         <v>9</v>
       </c>
@@ -10628,7 +10634,7 @@
       </c>
       <c r="AI7" s="99"/>
     </row>
-    <row r="8" spans="1:35" ht="24" customHeight="1">
+    <row r="8" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
@@ -10670,7 +10676,7 @@
       </c>
       <c r="AI8" s="100"/>
     </row>
-    <row r="9" spans="1:35" ht="24" customHeight="1">
+    <row r="9" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="32"/>
       <c r="C9" s="47"/>
@@ -10710,7 +10716,7 @@
       </c>
       <c r="AI9" s="100"/>
     </row>
-    <row r="10" spans="1:35" ht="24" customHeight="1">
+    <row r="10" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="32"/>
       <c r="C10" s="47"/>
@@ -10750,7 +10756,7 @@
       </c>
       <c r="AI10" s="100"/>
     </row>
-    <row r="11" spans="1:35" ht="24" customHeight="1">
+    <row r="11" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
       <c r="B11" s="32"/>
       <c r="C11" s="47"/>
@@ -10790,7 +10796,7 @@
       </c>
       <c r="AI11" s="100"/>
     </row>
-    <row r="12" spans="1:35" ht="24" customHeight="1">
+    <row r="12" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="51"/>
       <c r="C12" s="47"/>
@@ -10830,7 +10836,7 @@
       </c>
       <c r="AI12" s="100"/>
     </row>
-    <row r="13" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="13" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
         <v>11</v>
       </c>
@@ -10872,7 +10878,7 @@
       </c>
       <c r="AI13" s="100"/>
     </row>
-    <row r="14" spans="1:35" ht="24" customHeight="1">
+    <row r="14" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
         <v>13</v>
       </c>
@@ -10914,7 +10920,7 @@
       </c>
       <c r="AI14" s="100"/>
     </row>
-    <row r="15" spans="1:35" ht="24" customHeight="1">
+    <row r="15" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
         <v>12</v>
       </c>
@@ -10956,7 +10962,7 @@
       </c>
       <c r="AI15" s="100"/>
     </row>
-    <row r="16" spans="1:35" ht="24" customHeight="1">
+    <row r="16" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="32"/>
       <c r="C16" s="47"/>
@@ -10996,7 +11002,7 @@
       </c>
       <c r="AI16" s="100"/>
     </row>
-    <row r="17" spans="1:35" ht="24" customHeight="1">
+    <row r="17" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="32"/>
       <c r="C17" s="47"/>
@@ -11036,7 +11042,7 @@
       </c>
       <c r="AI17" s="100"/>
     </row>
-    <row r="18" spans="1:35" ht="24" customHeight="1">
+    <row r="18" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="32"/>
       <c r="C18" s="47"/>
@@ -11076,7 +11082,7 @@
       </c>
       <c r="AI18" s="100"/>
     </row>
-    <row r="19" spans="1:35" ht="24" customHeight="1">
+    <row r="19" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="32"/>
       <c r="C19" s="47"/>
@@ -11116,7 +11122,7 @@
       </c>
       <c r="AI19" s="100"/>
     </row>
-    <row r="20" spans="1:35" ht="24" customHeight="1">
+    <row r="20" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="51"/>
       <c r="C20" s="47"/>
@@ -11156,7 +11162,7 @@
       </c>
       <c r="AI20" s="100"/>
     </row>
-    <row r="21" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="21" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
         <v>15</v>
       </c>
@@ -11198,7 +11204,7 @@
       </c>
       <c r="AI21" s="100"/>
     </row>
-    <row r="22" spans="1:35" ht="24" customHeight="1">
+    <row r="22" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>16</v>
       </c>
@@ -11242,7 +11248,7 @@
       </c>
       <c r="AI22" s="100"/>
     </row>
-    <row r="23" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="23" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="43" t="s">
         <v>10</v>
@@ -11284,7 +11290,7 @@
       </c>
       <c r="AI23" s="100"/>
     </row>
-    <row r="24" spans="1:35" ht="24" customHeight="1">
+    <row r="24" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>17</v>
       </c>
@@ -11328,7 +11334,7 @@
       </c>
       <c r="AI24" s="100"/>
     </row>
-    <row r="25" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="25" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
       <c r="B25" s="43" t="s">
         <v>10</v>
@@ -11370,7 +11376,7 @@
       </c>
       <c r="AI25" s="100"/>
     </row>
-    <row r="26" spans="1:35" ht="24" customHeight="1">
+    <row r="26" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
         <v>18</v>
       </c>
@@ -11414,7 +11420,7 @@
       </c>
       <c r="AI26" s="100"/>
     </row>
-    <row r="27" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="27" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27" s="43" t="s">
         <v>10</v>
@@ -11456,7 +11462,7 @@
       </c>
       <c r="AI27" s="100"/>
     </row>
-    <row r="28" spans="1:35" ht="24" customHeight="1">
+    <row r="28" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="30"/>
       <c r="B28" s="44"/>
       <c r="C28" s="47"/>
@@ -11496,7 +11502,7 @@
       </c>
       <c r="AI28" s="100"/>
     </row>
-    <row r="29" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="29" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
       <c r="B29" s="43"/>
       <c r="C29" s="47"/>
@@ -11536,7 +11542,7 @@
       </c>
       <c r="AI29" s="100"/>
     </row>
-    <row r="30" spans="1:35" ht="24" customHeight="1">
+    <row r="30" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30"/>
       <c r="B30" s="44"/>
       <c r="C30" s="47"/>
@@ -11576,7 +11582,7 @@
       </c>
       <c r="AI30" s="100"/>
     </row>
-    <row r="31" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="31" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="B31" s="43"/>
       <c r="C31" s="47"/>
@@ -11616,7 +11622,7 @@
       </c>
       <c r="AI31" s="100"/>
     </row>
-    <row r="32" spans="1:35" ht="24" customHeight="1">
+    <row r="32" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="45"/>
       <c r="B32" s="44"/>
       <c r="C32" s="47"/>
@@ -11656,7 +11662,7 @@
       </c>
       <c r="AI32" s="100"/>
     </row>
-    <row r="33" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="33" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
       <c r="B33" s="43"/>
       <c r="C33" s="47"/>
@@ -11696,7 +11702,7 @@
       </c>
       <c r="AI33" s="100"/>
     </row>
-    <row r="34" spans="1:35" ht="24" customHeight="1">
+    <row r="34" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="45"/>
       <c r="B34" s="44"/>
       <c r="C34" s="47"/>
@@ -11736,7 +11742,7 @@
       </c>
       <c r="AI34" s="100"/>
     </row>
-    <row r="35" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="35" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
       <c r="B35" s="53"/>
       <c r="C35" s="47"/>
@@ -11776,7 +11782,7 @@
       </c>
       <c r="AI35" s="100"/>
     </row>
-    <row r="36" spans="1:35" ht="24" customHeight="1">
+    <row r="36" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="49"/>
       <c r="B36" s="44"/>
       <c r="C36" s="47"/>
@@ -11816,7 +11822,7 @@
       </c>
       <c r="AI36" s="100"/>
     </row>
-    <row r="37" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="37" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="B37" s="53"/>
       <c r="C37" s="47"/>
@@ -11856,7 +11862,7 @@
       </c>
       <c r="AI37" s="100"/>
     </row>
-    <row r="38" spans="1:35" ht="24" customHeight="1">
+    <row r="38" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="45"/>
       <c r="B38" s="44"/>
       <c r="C38" s="47"/>
@@ -11896,7 +11902,7 @@
       </c>
       <c r="AI38" s="100"/>
     </row>
-    <row r="39" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="39" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="53"/>
       <c r="C39" s="47"/>
@@ -11936,7 +11942,7 @@
       </c>
       <c r="AI39" s="100"/>
     </row>
-    <row r="40" spans="1:35" ht="24" customHeight="1">
+    <row r="40" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="13"/>
       <c r="B40" s="44"/>
       <c r="C40" s="47"/>
@@ -11976,7 +11982,7 @@
       </c>
       <c r="AI40" s="100"/>
     </row>
-    <row r="41" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="41" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31"/>
       <c r="B41" s="53"/>
       <c r="C41" s="47"/>
@@ -12016,7 +12022,7 @@
       </c>
       <c r="AI41" s="100"/>
     </row>
-    <row r="42" spans="1:35" ht="24" customHeight="1">
+    <row r="42" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13"/>
       <c r="B42" s="44"/>
       <c r="C42" s="47"/>
@@ -12056,7 +12062,7 @@
       </c>
       <c r="AI42" s="100"/>
     </row>
-    <row r="43" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="43" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31"/>
       <c r="B43" s="43"/>
       <c r="C43" s="47"/>
@@ -12096,7 +12102,7 @@
       </c>
       <c r="AI43" s="100"/>
     </row>
-    <row r="44" spans="1:35" ht="24" customHeight="1">
+    <row r="44" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="30"/>
       <c r="B44" s="44"/>
       <c r="C44" s="47"/>
@@ -12136,7 +12142,7 @@
       </c>
       <c r="AI44" s="100"/>
     </row>
-    <row r="45" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="45" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="43"/>
       <c r="C45" s="47"/>
@@ -12176,7 +12182,7 @@
       </c>
       <c r="AI45" s="100"/>
     </row>
-    <row r="46" spans="1:35" ht="24" customHeight="1">
+    <row r="46" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="49"/>
       <c r="B46" s="44"/>
       <c r="C46" s="47"/>
@@ -12216,7 +12222,7 @@
       </c>
       <c r="AI46" s="100"/>
     </row>
-    <row r="47" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="47" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="43"/>
       <c r="C47" s="47"/>
@@ -12256,7 +12262,7 @@
       </c>
       <c r="AI47" s="100"/>
     </row>
-    <row r="48" spans="1:35" ht="24" customHeight="1">
+    <row r="48" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="42"/>
       <c r="B48" s="44"/>
       <c r="C48" s="47"/>
@@ -12296,7 +12302,7 @@
       </c>
       <c r="AI48" s="100"/>
     </row>
-    <row r="49" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="49" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="43"/>
       <c r="C49" s="47"/>
@@ -12336,7 +12342,7 @@
       </c>
       <c r="AI49" s="100"/>
     </row>
-    <row r="50" spans="1:35" ht="24" customHeight="1">
+    <row r="50" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
       <c r="B50" s="30"/>
       <c r="C50" s="47"/>
@@ -12376,7 +12382,7 @@
       </c>
       <c r="AI50" s="100"/>
     </row>
-    <row r="51" spans="1:35" ht="24" customHeight="1">
+    <row r="51" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="47"/>
@@ -12416,7 +12422,7 @@
       </c>
       <c r="AI51" s="100"/>
     </row>
-    <row r="52" spans="1:35" ht="24" customHeight="1">
+    <row r="52" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="47"/>
@@ -12456,7 +12462,7 @@
       </c>
       <c r="AI52" s="100"/>
     </row>
-    <row r="53" spans="1:35" ht="24" customHeight="1">
+    <row r="53" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="47"/>
@@ -12496,7 +12502,7 @@
       </c>
       <c r="AI53" s="100"/>
     </row>
-    <row r="54" spans="1:35" ht="24" customHeight="1">
+    <row r="54" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="47"/>
@@ -12536,7 +12542,7 @@
       </c>
       <c r="AI54" s="100"/>
     </row>
-    <row r="55" spans="1:35" ht="24" customHeight="1">
+    <row r="55" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="47"/>
@@ -12576,7 +12582,7 @@
       </c>
       <c r="AI55" s="100"/>
     </row>
-    <row r="56" spans="1:35" ht="24" customHeight="1">
+    <row r="56" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="47"/>
@@ -12616,7 +12622,7 @@
       </c>
       <c r="AI56" s="100"/>
     </row>
-    <row r="57" spans="1:35" ht="24" customHeight="1">
+    <row r="57" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="47"/>
@@ -12656,7 +12662,7 @@
       </c>
       <c r="AI57" s="100"/>
     </row>
-    <row r="58" spans="1:35" ht="24" customHeight="1">
+    <row r="58" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="47"/>
@@ -12696,7 +12702,7 @@
       </c>
       <c r="AI58" s="100"/>
     </row>
-    <row r="59" spans="1:35" ht="24" customHeight="1">
+    <row r="59" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="13"/>
       <c r="B59" s="51"/>
       <c r="C59" s="47"/>
@@ -12736,7 +12742,7 @@
       </c>
       <c r="AI59" s="100"/>
     </row>
-    <row r="60" spans="1:35" ht="24" customHeight="1">
+    <row r="60" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="13"/>
       <c r="B60" s="51"/>
       <c r="C60" s="47"/>
@@ -12776,7 +12782,7 @@
       </c>
       <c r="AI60" s="100"/>
     </row>
-    <row r="61" spans="1:35" ht="24" customHeight="1">
+    <row r="61" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="13"/>
       <c r="B61" s="51"/>
       <c r="C61" s="47"/>
@@ -12816,7 +12822,7 @@
       </c>
       <c r="AI61" s="100"/>
     </row>
-    <row r="62" spans="1:35" ht="24" customHeight="1">
+    <row r="62" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="13"/>
       <c r="B62" s="51"/>
       <c r="C62" s="47"/>
@@ -12856,7 +12862,7 @@
       </c>
       <c r="AI62" s="100"/>
     </row>
-    <row r="63" spans="1:35" ht="24" customHeight="1">
+    <row r="63" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="13"/>
       <c r="B63" s="51"/>
       <c r="C63" s="47"/>
@@ -12896,7 +12902,7 @@
       </c>
       <c r="AI63" s="100"/>
     </row>
-    <row r="64" spans="1:35" ht="24" customHeight="1">
+    <row r="64" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="13"/>
       <c r="B64" s="51"/>
       <c r="C64" s="47"/>
@@ -12936,7 +12942,7 @@
       </c>
       <c r="AI64" s="100"/>
     </row>
-    <row r="65" spans="1:35" ht="24" customHeight="1">
+    <row r="65" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="13"/>
       <c r="B65" s="51"/>
       <c r="C65" s="47"/>
@@ -12976,7 +12982,7 @@
       </c>
       <c r="AI65" s="100"/>
     </row>
-    <row r="66" spans="1:35" ht="24" customHeight="1">
+    <row r="66" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="13"/>
       <c r="B66" s="51"/>
       <c r="C66" s="47"/>
@@ -13016,7 +13022,7 @@
       </c>
       <c r="AI66" s="100"/>
     </row>
-    <row r="67" spans="1:35" ht="24" customHeight="1">
+    <row r="67" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="13"/>
       <c r="B67" s="51"/>
       <c r="C67" s="47"/>
@@ -13056,7 +13062,7 @@
       </c>
       <c r="AI67" s="100"/>
     </row>
-    <row r="68" spans="1:35" ht="24" customHeight="1">
+    <row r="68" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="46"/>
       <c r="B68" s="46"/>
       <c r="C68" s="47"/>
@@ -13096,7 +13102,7 @@
       </c>
       <c r="AI68" s="100"/>
     </row>
-    <row r="69" spans="1:35" ht="24" customHeight="1">
+    <row r="69" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="46"/>
       <c r="B69" s="46"/>
       <c r="C69" s="47"/>
@@ -13136,7 +13142,7 @@
       </c>
       <c r="AI69" s="100"/>
     </row>
-    <row r="70" spans="1:35" ht="24" customHeight="1" thickBot="1">
+    <row r="70" spans="1:35" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="52" t="s">
         <v>19</v>
       </c>
@@ -13178,7 +13184,7 @@
       </c>
       <c r="AI70" s="100"/>
     </row>
-    <row r="71" spans="1:35" ht="24" customHeight="1">
+    <row r="71" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="42" t="s">
         <v>21</v>
       </c>
@@ -13222,7 +13228,7 @@
       </c>
       <c r="AI71" s="100"/>
     </row>
-    <row r="72" spans="1:35" ht="24" customHeight="1">
+    <row r="72" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="42" t="s">
         <v>22</v>
       </c>
@@ -13266,7 +13272,7 @@
       </c>
       <c r="AI72" s="100"/>
     </row>
-    <row r="73" spans="1:35" ht="24" customHeight="1">
+    <row r="73" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="42" t="s">
         <v>23</v>
       </c>
@@ -13310,7 +13316,7 @@
       </c>
       <c r="AI73" s="100"/>
     </row>
-    <row r="74" spans="1:35" ht="24" customHeight="1">
+    <row r="74" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="87"/>
       <c r="B74" s="32"/>
       <c r="C74" s="47"/>
@@ -13350,7 +13356,7 @@
       </c>
       <c r="AI74" s="100"/>
     </row>
-    <row r="75" spans="1:35" ht="24" customHeight="1">
+    <row r="75" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="49"/>
       <c r="B75" s="50"/>
       <c r="C75" s="47"/>
@@ -13390,7 +13396,7 @@
       </c>
       <c r="AI75" s="100"/>
     </row>
-    <row r="76" spans="1:35" ht="24" customHeight="1">
+    <row r="76" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="45"/>
       <c r="B76" s="50"/>
       <c r="C76" s="47"/>
@@ -13430,7 +13436,7 @@
       </c>
       <c r="AI76" s="100"/>
     </row>
-    <row r="77" spans="1:35" ht="24" customHeight="1">
+    <row r="77" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="70"/>
       <c r="B77" s="50"/>
       <c r="C77" s="47"/>
@@ -13470,7 +13476,7 @@
       </c>
       <c r="AI77" s="100"/>
     </row>
-    <row r="78" spans="1:35" ht="24" customHeight="1">
+    <row r="78" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="70"/>
       <c r="B78" s="50"/>
       <c r="C78" s="47"/>
@@ -13510,7 +13516,7 @@
       </c>
       <c r="AI78" s="100"/>
     </row>
-    <row r="79" spans="1:35" ht="24" customHeight="1">
+    <row r="79" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="87"/>
       <c r="B79" s="50"/>
       <c r="C79" s="47"/>
@@ -13550,7 +13556,7 @@
       </c>
       <c r="AI79" s="100"/>
     </row>
-    <row r="80" spans="1:35" ht="24" customHeight="1">
+    <row r="80" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="70"/>
       <c r="B80" s="50"/>
       <c r="C80" s="47"/>
@@ -13590,7 +13596,7 @@
       </c>
       <c r="AI80" s="100"/>
     </row>
-    <row r="81" spans="1:35" ht="24" customHeight="1">
+    <row r="81" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="70"/>
       <c r="B81" s="50"/>
       <c r="C81" s="47"/>
@@ -13630,7 +13636,7 @@
       </c>
       <c r="AI81" s="100"/>
     </row>
-    <row r="82" spans="1:35" ht="24" customHeight="1">
+    <row r="82" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="42"/>
       <c r="B82" s="50"/>
       <c r="C82" s="47"/>
@@ -13670,7 +13676,7 @@
       </c>
       <c r="AI82" s="100"/>
     </row>
-    <row r="83" spans="1:35" ht="24" customHeight="1">
+    <row r="83" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="42"/>
       <c r="B83" s="50"/>
       <c r="C83" s="47"/>
@@ -13710,7 +13716,7 @@
       </c>
       <c r="AI83" s="100"/>
     </row>
-    <row r="84" spans="1:35" ht="24" customHeight="1">
+    <row r="84" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="42"/>
       <c r="B84" s="50"/>
       <c r="C84" s="88"/>
@@ -13750,7 +13756,7 @@
       </c>
       <c r="AI84" s="100"/>
     </row>
-    <row r="85" spans="1:35" ht="24" customHeight="1">
+    <row r="85" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="49"/>
       <c r="B85" s="50"/>
       <c r="C85" s="47"/>
@@ -13790,7 +13796,7 @@
       </c>
       <c r="AI85" s="100"/>
     </row>
-    <row r="86" spans="1:35" ht="24" customHeight="1">
+    <row r="86" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="45"/>
       <c r="B86" s="50"/>
       <c r="C86" s="47"/>
@@ -13830,7 +13836,7 @@
       </c>
       <c r="AI86" s="100"/>
     </row>
-    <row r="87" spans="1:35" ht="24" customHeight="1">
+    <row r="87" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="70"/>
       <c r="B87" s="50"/>
       <c r="C87" s="47"/>
@@ -13870,7 +13876,7 @@
       </c>
       <c r="AI87" s="100"/>
     </row>
-    <row r="88" spans="1:35" ht="24" customHeight="1">
+    <row r="88" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="70"/>
       <c r="B88" s="50"/>
       <c r="C88" s="47"/>
@@ -13910,7 +13916,7 @@
       </c>
       <c r="AI88" s="100"/>
     </row>
-    <row r="89" spans="1:35" ht="24" customHeight="1">
+    <row r="89" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="70"/>
       <c r="B89" s="50"/>
       <c r="C89" s="47"/>
@@ -13950,7 +13956,7 @@
       </c>
       <c r="AI89" s="100"/>
     </row>
-    <row r="90" spans="1:35" ht="24" customHeight="1">
+    <row r="90" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="70"/>
       <c r="B90" s="50"/>
       <c r="C90" s="47"/>
@@ -13990,7 +13996,7 @@
       </c>
       <c r="AI90" s="100"/>
     </row>
-    <row r="91" spans="1:35" ht="24" customHeight="1">
+    <row r="91" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="13"/>
       <c r="B91" s="74"/>
       <c r="C91" s="47"/>
@@ -14030,7 +14036,7 @@
       </c>
       <c r="AI91" s="100"/>
     </row>
-    <row r="92" spans="1:35" ht="24" customHeight="1">
+    <row r="92" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="13"/>
       <c r="B92" s="74"/>
       <c r="C92" s="47"/>
@@ -14070,7 +14076,7 @@
       </c>
       <c r="AI92" s="100"/>
     </row>
-    <row r="93" spans="1:35" ht="24" customHeight="1">
+    <row r="93" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="13"/>
       <c r="B93" s="74"/>
       <c r="C93" s="47"/>
@@ -14110,7 +14116,7 @@
       </c>
       <c r="AI93" s="100"/>
     </row>
-    <row r="94" spans="1:35" ht="24" customHeight="1">
+    <row r="94" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="13"/>
       <c r="B94" s="74"/>
       <c r="C94" s="47"/>
@@ -14150,7 +14156,7 @@
       </c>
       <c r="AI94" s="100"/>
     </row>
-    <row r="95" spans="1:35" ht="24" customHeight="1">
+    <row r="95" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="13"/>
       <c r="B95" s="74"/>
       <c r="C95" s="47"/>
@@ -14190,7 +14196,7 @@
       </c>
       <c r="AI95" s="100"/>
     </row>
-    <row r="96" spans="1:35" ht="24" customHeight="1">
+    <row r="96" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="13"/>
       <c r="B96" s="74"/>
       <c r="C96" s="47"/>
@@ -14230,7 +14236,7 @@
       </c>
       <c r="AI96" s="100"/>
     </row>
-    <row r="97" spans="1:35" ht="24" customHeight="1">
+    <row r="97" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="13"/>
       <c r="B97" s="74"/>
       <c r="C97" s="47"/>
@@ -14270,7 +14276,7 @@
       </c>
       <c r="AI97" s="100"/>
     </row>
-    <row r="98" spans="1:35" ht="24" customHeight="1">
+    <row r="98" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="13"/>
       <c r="B98" s="74"/>
       <c r="C98" s="47"/>
@@ -14310,7 +14316,7 @@
       </c>
       <c r="AI98" s="100"/>
     </row>
-    <row r="99" spans="1:35" ht="24" customHeight="1">
+    <row r="99" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="13"/>
       <c r="B99" s="74"/>
       <c r="C99" s="47"/>
@@ -14350,7 +14356,7 @@
       </c>
       <c r="AI99" s="100"/>
     </row>
-    <row r="100" spans="1:35" ht="37.5" customHeight="1">
+    <row r="100" spans="1:35" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
         <v>0</v>
       </c>
@@ -14488,414 +14494,414 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:35">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A101" s="14"/>
       <c r="B101" s="15"/>
       <c r="AD101" s="1"/>
     </row>
-    <row r="102" spans="1:35">
+    <row r="102" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AD102" s="1"/>
     </row>
-    <row r="103" spans="1:35">
+    <row r="103" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AD103" s="1"/>
     </row>
-    <row r="104" spans="1:35">
+    <row r="104" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AD104" s="1"/>
     </row>
-    <row r="105" spans="1:35">
+    <row r="105" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AD105" s="1"/>
     </row>
-    <row r="106" spans="1:35">
+    <row r="106" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AD106" s="1"/>
     </row>
-    <row r="107" spans="1:35">
+    <row r="107" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AD107" s="1"/>
     </row>
-    <row r="108" spans="1:35">
+    <row r="108" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AD108" s="1"/>
     </row>
-    <row r="109" spans="1:35">
+    <row r="109" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AD109" s="1"/>
     </row>
-    <row r="110" spans="1:35">
+    <row r="110" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AD110" s="1"/>
     </row>
-    <row r="111" spans="1:35">
+    <row r="111" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AD111" s="1"/>
     </row>
-    <row r="112" spans="1:35">
+    <row r="112" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AD112" s="1"/>
     </row>
-    <row r="113" spans="30:30">
+    <row r="113" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD113" s="1"/>
     </row>
-    <row r="114" spans="30:30">
+    <row r="114" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD114" s="1"/>
     </row>
-    <row r="115" spans="30:30">
+    <row r="115" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD115" s="1"/>
     </row>
-    <row r="116" spans="30:30">
+    <row r="116" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD116" s="1"/>
     </row>
-    <row r="117" spans="30:30">
+    <row r="117" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD117" s="1"/>
     </row>
-    <row r="118" spans="30:30">
+    <row r="118" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD118" s="1"/>
     </row>
-    <row r="119" spans="30:30">
+    <row r="119" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD119" s="1"/>
     </row>
-    <row r="120" spans="30:30">
+    <row r="120" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD120" s="1"/>
     </row>
-    <row r="121" spans="30:30">
+    <row r="121" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD121" s="1"/>
     </row>
-    <row r="122" spans="30:30">
+    <row r="122" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD122" s="1"/>
     </row>
-    <row r="123" spans="30:30">
+    <row r="123" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD123" s="1"/>
     </row>
-    <row r="124" spans="30:30">
+    <row r="124" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD124" s="1"/>
     </row>
-    <row r="125" spans="30:30">
+    <row r="125" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD125" s="1"/>
     </row>
-    <row r="126" spans="30:30">
+    <row r="126" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD126" s="1"/>
     </row>
-    <row r="127" spans="30:30">
+    <row r="127" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD127" s="1"/>
     </row>
-    <row r="128" spans="30:30">
+    <row r="128" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD128" s="1"/>
     </row>
-    <row r="129" spans="30:30">
+    <row r="129" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD129" s="1"/>
     </row>
-    <row r="130" spans="30:30">
+    <row r="130" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD130" s="1"/>
     </row>
-    <row r="131" spans="30:30">
+    <row r="131" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD131" s="1"/>
     </row>
-    <row r="132" spans="30:30">
+    <row r="132" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD132" s="1"/>
     </row>
-    <row r="133" spans="30:30">
+    <row r="133" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD133" s="1"/>
     </row>
-    <row r="134" spans="30:30">
+    <row r="134" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD134" s="1"/>
     </row>
-    <row r="135" spans="30:30">
+    <row r="135" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD135" s="1"/>
     </row>
-    <row r="136" spans="30:30">
+    <row r="136" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD136" s="1"/>
     </row>
-    <row r="137" spans="30:30">
+    <row r="137" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD137" s="1"/>
     </row>
-    <row r="138" spans="30:30">
+    <row r="138" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD138" s="1"/>
     </row>
-    <row r="139" spans="30:30">
+    <row r="139" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD139" s="1"/>
     </row>
-    <row r="140" spans="30:30">
+    <row r="140" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD140" s="1"/>
     </row>
-    <row r="141" spans="30:30">
+    <row r="141" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD141" s="1"/>
     </row>
-    <row r="142" spans="30:30">
+    <row r="142" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD142" s="1"/>
     </row>
-    <row r="143" spans="30:30">
+    <row r="143" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD143" s="1"/>
     </row>
-    <row r="144" spans="30:30">
+    <row r="144" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD144" s="1"/>
     </row>
-    <row r="145" spans="30:30">
+    <row r="145" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD145" s="1"/>
     </row>
-    <row r="146" spans="30:30">
+    <row r="146" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD146" s="1"/>
     </row>
-    <row r="147" spans="30:30">
+    <row r="147" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD147" s="1"/>
     </row>
-    <row r="148" spans="30:30">
+    <row r="148" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD148" s="1"/>
     </row>
-    <row r="149" spans="30:30">
+    <row r="149" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD149" s="1"/>
     </row>
-    <row r="150" spans="30:30">
+    <row r="150" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD150" s="1"/>
     </row>
-    <row r="151" spans="30:30">
+    <row r="151" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD151" s="1"/>
     </row>
-    <row r="152" spans="30:30">
+    <row r="152" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD152" s="1"/>
     </row>
-    <row r="153" spans="30:30">
+    <row r="153" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD153" s="1"/>
     </row>
-    <row r="154" spans="30:30">
+    <row r="154" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD154" s="1"/>
     </row>
-    <row r="155" spans="30:30">
+    <row r="155" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD155" s="1"/>
     </row>
-    <row r="156" spans="30:30">
+    <row r="156" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD156" s="1"/>
     </row>
-    <row r="157" spans="30:30">
+    <row r="157" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD157" s="1"/>
     </row>
-    <row r="158" spans="30:30">
+    <row r="158" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD158" s="1"/>
     </row>
-    <row r="159" spans="30:30">
+    <row r="159" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD159" s="1"/>
     </row>
-    <row r="160" spans="30:30">
+    <row r="160" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD160" s="1"/>
     </row>
-    <row r="161" spans="30:30">
+    <row r="161" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD161" s="1"/>
     </row>
-    <row r="162" spans="30:30">
+    <row r="162" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD162" s="1"/>
     </row>
-    <row r="163" spans="30:30">
+    <row r="163" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD163" s="1"/>
     </row>
-    <row r="164" spans="30:30">
+    <row r="164" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD164" s="1"/>
     </row>
-    <row r="165" spans="30:30">
+    <row r="165" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD165" s="1"/>
     </row>
-    <row r="166" spans="30:30">
+    <row r="166" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD166" s="1"/>
     </row>
-    <row r="167" spans="30:30">
+    <row r="167" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD167" s="1"/>
     </row>
-    <row r="168" spans="30:30">
+    <row r="168" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD168" s="1"/>
     </row>
-    <row r="169" spans="30:30">
+    <row r="169" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD169" s="1"/>
     </row>
-    <row r="170" spans="30:30">
+    <row r="170" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD170" s="1"/>
     </row>
-    <row r="171" spans="30:30">
+    <row r="171" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD171" s="1"/>
     </row>
-    <row r="172" spans="30:30">
+    <row r="172" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD172" s="1"/>
     </row>
-    <row r="173" spans="30:30">
+    <row r="173" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD173" s="1"/>
     </row>
-    <row r="174" spans="30:30">
+    <row r="174" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD174" s="1"/>
     </row>
-    <row r="175" spans="30:30">
+    <row r="175" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD175" s="1"/>
     </row>
-    <row r="176" spans="30:30">
+    <row r="176" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD176" s="1"/>
     </row>
-    <row r="177" spans="30:30">
+    <row r="177" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD177" s="1"/>
     </row>
-    <row r="178" spans="30:30">
+    <row r="178" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD178" s="1"/>
     </row>
-    <row r="179" spans="30:30">
+    <row r="179" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD179" s="1"/>
     </row>
-    <row r="180" spans="30:30">
+    <row r="180" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD180" s="1"/>
     </row>
-    <row r="181" spans="30:30">
+    <row r="181" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD181" s="1"/>
     </row>
-    <row r="182" spans="30:30">
+    <row r="182" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD182" s="1"/>
     </row>
-    <row r="183" spans="30:30">
+    <row r="183" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD183" s="1"/>
     </row>
-    <row r="184" spans="30:30">
+    <row r="184" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD184" s="1"/>
     </row>
-    <row r="185" spans="30:30">
+    <row r="185" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD185" s="1"/>
     </row>
-    <row r="186" spans="30:30">
+    <row r="186" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD186" s="1"/>
     </row>
-    <row r="187" spans="30:30">
+    <row r="187" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD187" s="1"/>
     </row>
-    <row r="188" spans="30:30">
+    <row r="188" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD188" s="1"/>
     </row>
-    <row r="189" spans="30:30">
+    <row r="189" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD189" s="1"/>
     </row>
-    <row r="190" spans="30:30">
+    <row r="190" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD190" s="1"/>
     </row>
-    <row r="191" spans="30:30">
+    <row r="191" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD191" s="1"/>
     </row>
-    <row r="192" spans="30:30">
+    <row r="192" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD192" s="1"/>
     </row>
-    <row r="193" spans="30:30">
+    <row r="193" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD193" s="1"/>
     </row>
-    <row r="194" spans="30:30">
+    <row r="194" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD194" s="1"/>
     </row>
-    <row r="195" spans="30:30">
+    <row r="195" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD195" s="1"/>
     </row>
-    <row r="196" spans="30:30">
+    <row r="196" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD196" s="1"/>
     </row>
-    <row r="197" spans="30:30">
+    <row r="197" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD197" s="1"/>
     </row>
-    <row r="198" spans="30:30">
+    <row r="198" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD198" s="1"/>
     </row>
-    <row r="199" spans="30:30">
+    <row r="199" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD199" s="1"/>
     </row>
-    <row r="200" spans="30:30">
+    <row r="200" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD200" s="1"/>
     </row>
-    <row r="201" spans="30:30">
+    <row r="201" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD201" s="1"/>
     </row>
-    <row r="202" spans="30:30">
+    <row r="202" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD202" s="1"/>
     </row>
-    <row r="203" spans="30:30">
+    <row r="203" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD203" s="1"/>
     </row>
-    <row r="204" spans="30:30">
+    <row r="204" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD204" s="1"/>
     </row>
-    <row r="205" spans="30:30">
+    <row r="205" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD205" s="1"/>
     </row>
-    <row r="206" spans="30:30">
+    <row r="206" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD206" s="1"/>
     </row>
-    <row r="207" spans="30:30">
+    <row r="207" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD207" s="1"/>
     </row>
-    <row r="208" spans="30:30">
+    <row r="208" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD208" s="1"/>
     </row>
-    <row r="209" spans="30:30">
+    <row r="209" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD209" s="1"/>
     </row>
-    <row r="210" spans="30:30">
+    <row r="210" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD210" s="1"/>
     </row>
-    <row r="211" spans="30:30">
+    <row r="211" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD211" s="1"/>
     </row>
-    <row r="212" spans="30:30">
+    <row r="212" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD212" s="1"/>
     </row>
-    <row r="213" spans="30:30">
+    <row r="213" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD213" s="1"/>
     </row>
-    <row r="214" spans="30:30">
+    <row r="214" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD214" s="1"/>
     </row>
-    <row r="215" spans="30:30">
+    <row r="215" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD215" s="1"/>
     </row>
-    <row r="216" spans="30:30">
+    <row r="216" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD216" s="1"/>
     </row>
-    <row r="217" spans="30:30">
+    <row r="217" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD217" s="1"/>
     </row>
-    <row r="218" spans="30:30">
+    <row r="218" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD218" s="1"/>
     </row>
-    <row r="219" spans="30:30">
+    <row r="219" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD219" s="1"/>
     </row>
-    <row r="220" spans="30:30">
+    <row r="220" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD220" s="1"/>
     </row>
-    <row r="221" spans="30:30">
+    <row r="221" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD221" s="1"/>
     </row>
-    <row r="222" spans="30:30">
+    <row r="222" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD222" s="1"/>
     </row>
-    <row r="223" spans="30:30">
+    <row r="223" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD223" s="1"/>
     </row>
-    <row r="224" spans="30:30">
+    <row r="224" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD224" s="1"/>
     </row>
-    <row r="225" spans="30:30">
+    <row r="225" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD225" s="1"/>
     </row>
-    <row r="226" spans="30:30">
+    <row r="226" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD226" s="1"/>
     </row>
-    <row r="227" spans="30:30">
+    <row r="227" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD227" s="1"/>
     </row>
-    <row r="228" spans="30:30">
+    <row r="228" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD228" s="1"/>
     </row>
-    <row r="229" spans="30:30">
+    <row r="229" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD229" s="1"/>
     </row>
-    <row r="230" spans="30:30">
+    <row r="230" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD230" s="1"/>
     </row>
-    <row r="231" spans="30:30">
+    <row r="231" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD231" s="1"/>
     </row>
-    <row r="232" spans="30:30">
+    <row r="232" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD232" s="1"/>
     </row>
-    <row r="233" spans="30:30">
+    <row r="233" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD233" s="1"/>
     </row>
-    <row r="234" spans="30:30">
+    <row r="234" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD234" s="1"/>
     </row>
-    <row r="235" spans="30:30">
+    <row r="235" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD235" s="1"/>
     </row>
-    <row r="236" spans="30:30">
+    <row r="236" spans="30:30" x14ac:dyDescent="0.2">
       <c r="AD236" s="1"/>
     </row>
   </sheetData>
@@ -14937,193 +14943,193 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="16"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="16"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>

</xml_diff>